<commit_message>
logistics .md with links to shipment and labeling scheme information
</commit_message>
<xml_diff>
--- a/admin/shipments/Shipments.xlsx
+++ b/admin/shipments/Shipments.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/admin/shipments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E14CE0-94D7-3040-ABEF-86777F5A5A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF7A5F4-804B-434E-8329-EE45FC7088BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{ED9BC409-34AF-8E4E-B4DF-C9B915733B34}"/>
+    <workbookView xWindow="5540" yWindow="460" windowWidth="28060" windowHeight="18960" xr2:uid="{ED9BC409-34AF-8E4E-B4DF-C9B915733B34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Shipment Date</t>
   </si>
@@ -64,6 +67,63 @@
   </si>
   <si>
     <t>UPenn</t>
+  </si>
+  <si>
+    <t>January 11th, 2022</t>
+  </si>
+  <si>
+    <t>Shipping Tech</t>
+  </si>
+  <si>
+    <t>Receiving Tech</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Lulu</t>
+  </si>
+  <si>
+    <t>Putnam lab grey large shipper</t>
+  </si>
+  <si>
+    <t>March 2021 physiology fragments, October November 2020 mixed molecular/physiology samples, November 2020  physiology ("T2") fragments, 3 fragments from June 2021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emma </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Dempsey (Emma's friend) transporting putnam lab grey large shipper from UPenn to URI and transporting blue Barott lab dry shipper from URI to UPenn. Both empty, no samples or LN2</t>
+  </si>
+  <si>
+    <t>September 28th, 2021</t>
+  </si>
+  <si>
+    <t>UH</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Wes</t>
+  </si>
+  <si>
+    <t>August 27 2020 molecular, August 27 2020 physiology fragments, December 2019 biopsy (molecular)</t>
+  </si>
+  <si>
+    <t>Emma can only find one set of August 2020 samples at URI. Other is missing. The shipment made it to URI because we have the 2/3 timepoints from this shipment.</t>
+  </si>
+  <si>
+    <t>January 25th, 2020</t>
+  </si>
+  <si>
+    <t>October 2020 biopsy, October 2020 physio, November 2020 biopsy, November 2020 phyio, falcon tube (Porites 6 Eva Majerova)</t>
+  </si>
+  <si>
+    <t>1.) Is this the right shipment date? 2.) plastic bags popped in transit and individuals whirlpaks not labeled 3.) Falcon tube not related to HI Bleaching Pairs project</t>
   </si>
 </sst>
 </file>
@@ -87,15 +147,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,13 +169,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2A3FFA-EAB1-674A-8568-AB23DA317931}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,44 +514,141 @@
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="45" customWidth="1"/>
+    <col min="5" max="5" width="71.5" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="76.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" t="s">
         <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{9E2A3FFA-EAB1-674A-8568-AB23DA317931}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
shipment details april 2022 and physiology URI labwork
</commit_message>
<xml_diff>
--- a/admin/shipments/Shipments.xlsx
+++ b/admin/shipments/Shipments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/admin/shipments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF7A5F4-804B-434E-8329-EE45FC7088BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBABE86F-6EBA-F049-B488-A4B3BA025DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5540" yWindow="460" windowWidth="28060" windowHeight="18960" xr2:uid="{ED9BC409-34AF-8E4E-B4DF-C9B915733B34}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Shipment Date</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>1.) Is this the right shipment date? 2.) plastic bags popped in transit and individuals whirlpaks not labeled 3.) Falcon tube not related to HI Bleaching Pairs project</t>
+  </si>
+  <si>
+    <t>April 26th, 2022</t>
+  </si>
+  <si>
+    <t>August 2020 fragments that have been clipped</t>
+  </si>
+  <si>
+    <t>UPenn shipping empty dry shipper back on May 2nd, 2022</t>
   </si>
 </sst>
 </file>
@@ -503,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2A3FFA-EAB1-674A-8568-AB23DA317931}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,6 +656,32 @@
         <v>19</v>
       </c>
     </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{9E2A3FFA-EAB1-674A-8568-AB23DA317931}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
shipments tracking for sperm samples sent to UPenn
</commit_message>
<xml_diff>
--- a/admin/shipments/Shipments.xlsx
+++ b/admin/shipments/Shipments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/admin/shipments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580E5217-7079-D54F-B58A-E710E4B8F10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C19EB6-A8D7-4B41-BF88-2186039E9F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5540" yWindow="460" windowWidth="28060" windowHeight="18960" xr2:uid="{ED9BC409-34AF-8E4E-B4DF-C9B915733B34}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Shipment Date</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>38 molecular biopsy fragments -- 2 may still be at UPENN?</t>
+  </si>
+  <si>
+    <t>October 18th, 2022</t>
+  </si>
+  <si>
+    <t>5 Acropora sperm samples in shield</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2A3FFA-EAB1-674A-8568-AB23DA317931}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,6 +726,32 @@
         <v>35</v>
       </c>
     </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{9E2A3FFA-EAB1-674A-8568-AB23DA317931}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>